<commit_message>
#2 starting to generalize to more contexts/dates.
</commit_message>
<xml_diff>
--- a/input_files/acfrs/example2.xlsx
+++ b/input_files/acfrs/example2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katrinawheelan/Desktop/Code/CLOSUP/process_xbrl/process-xbrl/input_files/afcrs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katrinawheelan/Desktop/Code/CLOSUP/process_xbrl/process-xbrl/input_files/acfrs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21E49F74-3499-B344-8200-E9FFE1CCCE94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B3C09D8-35DD-1E4D-B632-E96398316613}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1960" yWindow="1080" windowWidth="25200" windowHeight="14360" tabRatio="834" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1960" yWindow="1080" windowWidth="25200" windowHeight="14360" tabRatio="834" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Statement of Net Position" sheetId="1" r:id="rId1"/>
@@ -4153,7 +4153,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -4436,8 +4436,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4759,8 +4759,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>